<commit_message>
directory was cleaned up
</commit_message>
<xml_diff>
--- a/src/sbe_vallib/table/pipelines/Config_31.xlsx
+++ b/src/sbe_vallib/table/pipelines/Config_31.xlsx
@@ -7,12 +7,17 @@
     <sheet state="visible" name="agg_config" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_14A2CAD9_9538_4B1B_A607_B8C1E3BE611A_.wvu.FilterData">tests_config!$A$1:$AD$1000</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_31747976_AC6B_4DCE_B9DB_52755BC9FF3B_.wvu.FilterData">tests_config!$A$1:$AD$220</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{14A2CAD9-9538-4B1B-A607-B8C1E3BE611A}" name="Фильтр 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{31747976-AC6B-4DCE-B9DB-52755BC9FF3B}" name="Фильтр 1"/>
   </customWorkbookViews>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miLdJztcpPKqXR8TX+8D/X5CzcReg=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -55,7 +60,7 @@
     <t>params</t>
   </si>
   <si>
-    <t>sbe_vallib.validation.table.general_tests.data_quality.test_psi_factor.test_factor_psi</t>
+    <t>sbe_vallib.table.data_quality.test_psi_factor.test_factor_psi</t>
   </si>
   <si>
     <t>test_factor_psi</t>
@@ -89,7 +94,7 @@
  "threshold": (0.2, 10000000)}</t>
   </si>
   <si>
-    <t>sbe_vallib.validation.table.general_tests.model_quality.test_ci</t>
+    <t>sbe_vallib.table.model_quality.test_ci.test_ci</t>
   </si>
   <si>
     <t>test_ci</t>
@@ -179,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -187,17 +192,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -449,7 +451,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -464,97 +466,97 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" ht="88.5" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>0.0</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
     </row>
     <row r="3" ht="75.0" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.0</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>28</v>
       </c>
       <c r="I3" s="5"/>
@@ -563,24 +565,24 @@
       <c r="L3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
     </row>
     <row r="4" ht="75.0" customHeight="1">
       <c r="A4" s="5"/>
@@ -591,28 +593,28 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="8"/>
+      <c r="I4" s="7"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
     </row>
     <row r="5" ht="75.0" customHeight="1">
       <c r="A5" s="5"/>
@@ -623,28 +625,28 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="8"/>
+      <c r="I5" s="7"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
     </row>
     <row r="6" ht="61.5" customHeight="1">
       <c r="A6" s="5"/>
@@ -659,24 +661,24 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
     </row>
     <row r="7" ht="61.5" customHeight="1">
       <c r="A7" s="5"/>
@@ -691,24 +693,24 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7"/>
-      <c r="AD7" s="7"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
     </row>
     <row r="8" ht="75.0" customHeight="1">
       <c r="A8" s="5"/>
@@ -723,24 +725,24 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
     </row>
     <row r="9" ht="75.0" customHeight="1">
       <c r="A9" s="5"/>
@@ -755,39 +757,39 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="7"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
     </row>
     <row r="10" ht="75.0" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="7"/>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" ht="157.5" customHeight="1">
       <c r="A11" s="5"/>
@@ -802,39 +804,39 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="7"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
     </row>
     <row r="12" ht="61.5" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="9"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="5"/>
-      <c r="M12" s="7"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" ht="88.5" customHeight="1">
       <c r="A13" s="5"/>
@@ -849,24 +851,24 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="7"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
     </row>
     <row r="14" ht="61.5" customHeight="1">
       <c r="A14" s="5"/>
@@ -881,24 +883,24 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7"/>
-      <c r="AD14" s="7"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
     </row>
     <row r="15" ht="116.25" customHeight="1">
       <c r="A15" s="5"/>
@@ -913,24 +915,24 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="7"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
     </row>
     <row r="16" ht="116.25" customHeight="1">
       <c r="A16" s="5"/>
@@ -945,24 +947,24 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="7"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="7"/>
-      <c r="AD16" s="7"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
     </row>
     <row r="17" ht="116.25" customHeight="1">
       <c r="A17" s="5"/>
@@ -977,24 +979,24 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
-      <c r="AA17" s="7"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
     </row>
     <row r="18" ht="61.5" customHeight="1">
       <c r="A18" s="5"/>
@@ -1009,24 +1011,24 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
-      <c r="AA18" s="7"/>
-      <c r="AB18" s="7"/>
-      <c r="AC18" s="7"/>
-      <c r="AD18" s="7"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
     </row>
     <row r="19" ht="88.5" customHeight="1">
       <c r="A19" s="5"/>
@@ -1037,11 +1039,11 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="8"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="9"/>
+      <c r="K19" s="8"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="4"/>
+      <c r="M19" s="3"/>
     </row>
     <row r="20" ht="102.75" customHeight="1">
       <c r="A20" s="5"/>
@@ -1056,7 +1058,7 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="7"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" ht="19.5" customHeight="1"/>
     <row r="22" ht="19.5" customHeight="1"/>
@@ -2040,8 +2042,13 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{14A2CAD9-9538-4B1B-A607-B8C1E3BE611A}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$A$1:$AD$1000"/>
+    <customSheetView guid="{31747976-AC6B-4DCE-B9DB-52755BC9FF3B}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$A$1:$AD$220"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1819065991"/>
+        </ext>
+      </extLst>
     </customSheetView>
   </customSheetViews>
   <printOptions/>
@@ -2067,18 +2074,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2086,7 +2093,7 @@
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2094,7 +2101,7 @@
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2102,7 +2109,7 @@
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2110,7 +2117,7 @@
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>